<commit_message>
IMPLEMENTACION DE METODOS Y SERVICIOS PARA GUARDAR VENTA, ADEMAS SE CREO ENTIDADES COMO VENTA Y DETALLEVENTA || RETO 15 REGISTRAR VENTA ||funciona ok
</commit_message>
<xml_diff>
--- a/Base de Datos/01DiseñoBDD.xlsx
+++ b/Base de Datos/01DiseñoBDD.xlsx
@@ -3,12 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27932"/>
   <workbookPr defaultThemeVersion="202300"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ESCUELAPROGRAMACIONKD\03MODULO\inventarios\Base de Datos\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0984D188-101D-4CAB-9EA6-46FB054CE194}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{E66D6FF7-F3F1-4E32-88E1-CD566CDD7867}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{E9E292EC-47DE-4FD1-BDC6-A5B6D9350F58}"/>
   </bookViews>
@@ -17,6 +12,7 @@
     <sheet name="SERVICIOS" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -40,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="124">
   <si>
     <t>CATEGORIAS</t>
   </si>
@@ -396,9 +392,6 @@
     <t>/pedidos/registrar</t>
   </si>
   <si>
-    <t>crear cabecera del pedido</t>
-  </si>
-  <si>
     <t>PUT</t>
   </si>
   <si>
@@ -406,6 +399,15 @@
   </si>
   <si>
     <t>modificar el estado del pedido y de cada detalle actualiza la cantidad recibida y el subtotal.</t>
+  </si>
+  <si>
+    <t>/ventas/guardar</t>
+  </si>
+  <si>
+    <t>crear cabecera del pedido y el detalles del pedido</t>
+  </si>
+  <si>
+    <t>crear cabecera de la venta y el detalles de la venta</t>
   </si>
 </sst>
 </file>
@@ -753,28 +755,28 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1140,11 +1142,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B2" s="39" t="s">
+      <c r="B2" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B3" s="8" t="s">
@@ -1235,15 +1237,15 @@
       </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C12" s="40" t="s">
+      <c r="C12" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="41"/>
+      <c r="D12" s="43"/>
       <c r="E12" s="42"/>
-      <c r="G12" s="39" t="s">
+      <c r="G12" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="H12" s="39"/>
+      <c r="H12" s="44"/>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C13" s="8" t="s">
@@ -1364,16 +1366,16 @@
       </c>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B23" s="45" t="s">
+      <c r="B23" s="39" t="s">
         <v>38</v>
       </c>
-      <c r="C23" s="46"/>
-      <c r="D23" s="46"/>
-      <c r="E23" s="46"/>
-      <c r="F23" s="46"/>
-      <c r="G23" s="46"/>
-      <c r="H23" s="46"/>
-      <c r="I23" s="46"/>
+      <c r="C23" s="40"/>
+      <c r="D23" s="40"/>
+      <c r="E23" s="40"/>
+      <c r="F23" s="40"/>
+      <c r="G23" s="40"/>
+      <c r="H23" s="40"/>
+      <c r="I23" s="40"/>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B24" s="8" t="s">
@@ -1506,10 +1508,10 @@
       </c>
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C31" s="39" t="s">
+      <c r="C31" s="44" t="s">
         <v>46</v>
       </c>
-      <c r="D31" s="39"/>
+      <c r="D31" s="44"/>
     </row>
     <row r="32" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C32" s="8" t="s">
@@ -1536,14 +1538,14 @@
       </c>
     </row>
     <row r="36" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B36" s="39" t="s">
+      <c r="B36" s="44" t="s">
         <v>50</v>
       </c>
-      <c r="C36" s="39"/>
-      <c r="D36" s="39"/>
-      <c r="E36" s="39"/>
-      <c r="F36" s="39"/>
-      <c r="G36" s="39"/>
+      <c r="C36" s="44"/>
+      <c r="D36" s="44"/>
+      <c r="E36" s="44"/>
+      <c r="F36" s="44"/>
+      <c r="G36" s="44"/>
     </row>
     <row r="37" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B37" s="8" t="s">
@@ -1606,13 +1608,13 @@
       </c>
     </row>
     <row r="42" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B42" s="43" t="s">
+      <c r="B42" s="45" t="s">
         <v>70</v>
       </c>
-      <c r="C42" s="44"/>
-      <c r="D42" s="44"/>
-      <c r="E42" s="44"/>
-      <c r="I42" s="40" t="s">
+      <c r="C42" s="46"/>
+      <c r="D42" s="46"/>
+      <c r="E42" s="46"/>
+      <c r="I42" s="41" t="s">
         <v>80</v>
       </c>
       <c r="J42" s="42"/>
@@ -1678,14 +1680,14 @@
       </c>
     </row>
     <row r="47" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B47" s="39" t="s">
+      <c r="B47" s="44" t="s">
         <v>71</v>
       </c>
-      <c r="C47" s="39"/>
-      <c r="D47" s="39"/>
-      <c r="E47" s="39"/>
-      <c r="F47" s="39"/>
-      <c r="G47" s="39"/>
+      <c r="C47" s="44"/>
+      <c r="D47" s="44"/>
+      <c r="E47" s="44"/>
+      <c r="F47" s="44"/>
+      <c r="G47" s="44"/>
     </row>
     <row r="48" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B48" s="8" t="s">
@@ -1776,12 +1778,12 @@
       <c r="G52" s="2"/>
     </row>
     <row r="54" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B54" s="40" t="s">
+      <c r="B54" s="41" t="s">
         <v>85</v>
       </c>
-      <c r="C54" s="41"/>
-      <c r="D54" s="41"/>
-      <c r="E54" s="41"/>
+      <c r="C54" s="43"/>
+      <c r="D54" s="43"/>
+      <c r="E54" s="43"/>
       <c r="F54" s="42"/>
     </row>
     <row r="55" spans="2:8" x14ac:dyDescent="0.25">
@@ -1896,12 +1898,12 @@
       </c>
     </row>
     <row r="64" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B64" s="40" t="s">
+      <c r="B64" s="41" t="s">
         <v>90</v>
       </c>
-      <c r="C64" s="41"/>
-      <c r="D64" s="41"/>
-      <c r="E64" s="41"/>
+      <c r="C64" s="43"/>
+      <c r="D64" s="43"/>
+      <c r="E64" s="43"/>
       <c r="F64" s="42"/>
     </row>
     <row r="65" spans="2:9" x14ac:dyDescent="0.25">
@@ -1939,15 +1941,15 @@
       </c>
     </row>
     <row r="69" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B69" s="45" t="s">
+      <c r="B69" s="39" t="s">
         <v>94</v>
       </c>
-      <c r="C69" s="46"/>
-      <c r="D69" s="46"/>
-      <c r="E69" s="46"/>
-      <c r="F69" s="46"/>
-      <c r="G69" s="46"/>
-      <c r="H69" s="46"/>
+      <c r="C69" s="40"/>
+      <c r="D69" s="40"/>
+      <c r="E69" s="40"/>
+      <c r="F69" s="40"/>
+      <c r="G69" s="40"/>
+      <c r="H69" s="40"/>
     </row>
     <row r="70" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B70" s="8" t="s">
@@ -2041,6 +2043,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="C12:E12"/>
+    <mergeCell ref="B47:G47"/>
+    <mergeCell ref="B42:E42"/>
     <mergeCell ref="B69:H69"/>
     <mergeCell ref="I42:J42"/>
     <mergeCell ref="B23:I23"/>
@@ -2048,11 +2055,6 @@
     <mergeCell ref="B64:F64"/>
     <mergeCell ref="C31:D31"/>
     <mergeCell ref="B36:G36"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="C12:E12"/>
-    <mergeCell ref="B47:G47"/>
-    <mergeCell ref="B42:E42"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
@@ -2069,7 +2071,7 @@
   <dimension ref="B2:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2161,24 +2163,30 @@
         <v>117</v>
       </c>
       <c r="D9" s="36" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
     </row>
     <row r="10" spans="2:5" s="35" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B10" s="36" t="s">
+        <v>118</v>
+      </c>
+      <c r="C10" s="36" t="s">
         <v>119</v>
       </c>
-      <c r="C10" s="36" t="s">
+      <c r="D10" s="36" t="s">
         <v>120</v>
       </c>
-      <c r="D10" s="36" t="s">
+    </row>
+    <row r="11" spans="2:5" s="35" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B11" s="36" t="s">
+        <v>114</v>
+      </c>
+      <c r="C11" s="36" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="11" spans="2:5" s="35" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B11" s="36"/>
-      <c r="C11" s="36"/>
-      <c r="D11" s="36"/>
+      <c r="D11" s="36" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="12" spans="2:5" s="35" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B12" s="36"/>

</xml_diff>

<commit_message>
IMPLEMENTACION DE METODOS Y SERVICIO DE ACTUALIZAR PRODUCTO || RETO 16 SERVICIOS VARIOS||funciona ok
</commit_message>
<xml_diff>
--- a/Base de Datos/01DiseñoBDD.xlsx
+++ b/Base de Datos/01DiseñoBDD.xlsx
@@ -3,7 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27932"/>
   <workbookPr defaultThemeVersion="202300"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{E66D6FF7-F3F1-4E32-88E1-CD566CDD7867}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ESCUELAPROGRAMACIONKD\03MODULO\inventarios\Base de Datos\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DD4D54E-34B2-4398-9B15-B0675978E4C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{E9E292EC-47DE-4FD1-BDC6-A5B6D9350F58}"/>
   </bookViews>
@@ -12,7 +17,6 @@
     <sheet name="SERVICIOS" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="126">
   <si>
     <t>CATEGORIAS</t>
   </si>
@@ -374,9 +378,6 @@
     <t>crea o inserta un nuevo proveedor</t>
   </si>
   <si>
-    <t>/produsctos/buscar/{subcadena}</t>
-  </si>
-  <si>
     <t>recupera todos los productos cuyo nombre contenga la subcadena con el path param</t>
   </si>
   <si>
@@ -408,6 +409,15 @@
   </si>
   <si>
     <t>crear cabecera de la venta y el detalles de la venta</t>
+  </si>
+  <si>
+    <t>/productos/buscar/{subcadena}</t>
+  </si>
+  <si>
+    <t>/productos/actualizar</t>
+  </si>
+  <si>
+    <t>actualiza o modifica un producto de acuerdo a la id</t>
   </si>
 </sst>
 </file>
@@ -755,28 +765,28 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1142,11 +1152,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B2" s="44" t="s">
+      <c r="B2" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B3" s="8" t="s">
@@ -1237,15 +1247,15 @@
       </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C12" s="41" t="s">
+      <c r="C12" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="43"/>
+      <c r="D12" s="41"/>
       <c r="E12" s="42"/>
-      <c r="G12" s="44" t="s">
+      <c r="G12" s="39" t="s">
         <v>14</v>
       </c>
-      <c r="H12" s="44"/>
+      <c r="H12" s="39"/>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C13" s="8" t="s">
@@ -1366,16 +1376,16 @@
       </c>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B23" s="39" t="s">
+      <c r="B23" s="45" t="s">
         <v>38</v>
       </c>
-      <c r="C23" s="40"/>
-      <c r="D23" s="40"/>
-      <c r="E23" s="40"/>
-      <c r="F23" s="40"/>
-      <c r="G23" s="40"/>
-      <c r="H23" s="40"/>
-      <c r="I23" s="40"/>
+      <c r="C23" s="46"/>
+      <c r="D23" s="46"/>
+      <c r="E23" s="46"/>
+      <c r="F23" s="46"/>
+      <c r="G23" s="46"/>
+      <c r="H23" s="46"/>
+      <c r="I23" s="46"/>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B24" s="8" t="s">
@@ -1508,10 +1518,10 @@
       </c>
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C31" s="44" t="s">
+      <c r="C31" s="39" t="s">
         <v>46</v>
       </c>
-      <c r="D31" s="44"/>
+      <c r="D31" s="39"/>
     </row>
     <row r="32" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C32" s="8" t="s">
@@ -1538,14 +1548,14 @@
       </c>
     </row>
     <row r="36" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B36" s="44" t="s">
+      <c r="B36" s="39" t="s">
         <v>50</v>
       </c>
-      <c r="C36" s="44"/>
-      <c r="D36" s="44"/>
-      <c r="E36" s="44"/>
-      <c r="F36" s="44"/>
-      <c r="G36" s="44"/>
+      <c r="C36" s="39"/>
+      <c r="D36" s="39"/>
+      <c r="E36" s="39"/>
+      <c r="F36" s="39"/>
+      <c r="G36" s="39"/>
     </row>
     <row r="37" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B37" s="8" t="s">
@@ -1608,13 +1618,13 @@
       </c>
     </row>
     <row r="42" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B42" s="45" t="s">
+      <c r="B42" s="43" t="s">
         <v>70</v>
       </c>
-      <c r="C42" s="46"/>
-      <c r="D42" s="46"/>
-      <c r="E42" s="46"/>
-      <c r="I42" s="41" t="s">
+      <c r="C42" s="44"/>
+      <c r="D42" s="44"/>
+      <c r="E42" s="44"/>
+      <c r="I42" s="40" t="s">
         <v>80</v>
       </c>
       <c r="J42" s="42"/>
@@ -1680,14 +1690,14 @@
       </c>
     </row>
     <row r="47" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B47" s="44" t="s">
+      <c r="B47" s="39" t="s">
         <v>71</v>
       </c>
-      <c r="C47" s="44"/>
-      <c r="D47" s="44"/>
-      <c r="E47" s="44"/>
-      <c r="F47" s="44"/>
-      <c r="G47" s="44"/>
+      <c r="C47" s="39"/>
+      <c r="D47" s="39"/>
+      <c r="E47" s="39"/>
+      <c r="F47" s="39"/>
+      <c r="G47" s="39"/>
     </row>
     <row r="48" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B48" s="8" t="s">
@@ -1778,12 +1788,12 @@
       <c r="G52" s="2"/>
     </row>
     <row r="54" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B54" s="41" t="s">
+      <c r="B54" s="40" t="s">
         <v>85</v>
       </c>
-      <c r="C54" s="43"/>
-      <c r="D54" s="43"/>
-      <c r="E54" s="43"/>
+      <c r="C54" s="41"/>
+      <c r="D54" s="41"/>
+      <c r="E54" s="41"/>
       <c r="F54" s="42"/>
     </row>
     <row r="55" spans="2:8" x14ac:dyDescent="0.25">
@@ -1898,12 +1908,12 @@
       </c>
     </row>
     <row r="64" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B64" s="41" t="s">
+      <c r="B64" s="40" t="s">
         <v>90</v>
       </c>
-      <c r="C64" s="43"/>
-      <c r="D64" s="43"/>
-      <c r="E64" s="43"/>
+      <c r="C64" s="41"/>
+      <c r="D64" s="41"/>
+      <c r="E64" s="41"/>
       <c r="F64" s="42"/>
     </row>
     <row r="65" spans="2:9" x14ac:dyDescent="0.25">
@@ -1941,15 +1951,15 @@
       </c>
     </row>
     <row r="69" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B69" s="39" t="s">
+      <c r="B69" s="45" t="s">
         <v>94</v>
       </c>
-      <c r="C69" s="40"/>
-      <c r="D69" s="40"/>
-      <c r="E69" s="40"/>
-      <c r="F69" s="40"/>
-      <c r="G69" s="40"/>
-      <c r="H69" s="40"/>
+      <c r="C69" s="46"/>
+      <c r="D69" s="46"/>
+      <c r="E69" s="46"/>
+      <c r="F69" s="46"/>
+      <c r="G69" s="46"/>
+      <c r="H69" s="46"/>
     </row>
     <row r="70" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B70" s="8" t="s">
@@ -2043,11 +2053,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="C12:E12"/>
-    <mergeCell ref="B47:G47"/>
-    <mergeCell ref="B42:E42"/>
     <mergeCell ref="B69:H69"/>
     <mergeCell ref="I42:J42"/>
     <mergeCell ref="B23:I23"/>
@@ -2055,6 +2060,11 @@
     <mergeCell ref="B64:F64"/>
     <mergeCell ref="C31:D31"/>
     <mergeCell ref="B36:G36"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="C12:E12"/>
+    <mergeCell ref="B47:G47"/>
+    <mergeCell ref="B42:E42"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
@@ -2071,7 +2081,7 @@
   <dimension ref="B2:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2138,60 +2148,66 @@
         <v>102</v>
       </c>
       <c r="C7" s="36" t="s">
+        <v>123</v>
+      </c>
+      <c r="D7" s="36" t="s">
         <v>112</v>
-      </c>
-      <c r="D7" s="36" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="8" spans="2:5" s="35" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B8" s="36" t="s">
+        <v>113</v>
+      </c>
+      <c r="C8" s="36" t="s">
         <v>114</v>
       </c>
-      <c r="C8" s="36" t="s">
+      <c r="D8" s="36" t="s">
         <v>115</v>
-      </c>
-      <c r="D8" s="36" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="9" spans="2:5" s="35" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B9" s="36" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C9" s="36" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D9" s="36" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="10" spans="2:5" s="35" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B10" s="36" t="s">
+        <v>117</v>
+      </c>
+      <c r="C10" s="36" t="s">
         <v>118</v>
       </c>
-      <c r="C10" s="36" t="s">
+      <c r="D10" s="36" t="s">
         <v>119</v>
-      </c>
-      <c r="D10" s="36" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="11" spans="2:5" s="35" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B11" s="36" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C11" s="36" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D11" s="36" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="12" spans="2:5" s="35" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B12" s="36"/>
-      <c r="C12" s="36"/>
-      <c r="D12" s="36"/>
+      <c r="B12" s="36" t="s">
+        <v>117</v>
+      </c>
+      <c r="C12" s="36" t="s">
+        <v>124</v>
+      </c>
+      <c r="D12" s="36" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="13" spans="2:5" s="35" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B13" s="36"/>
@@ -2200,7 +2216,7 @@
     </row>
     <row r="14" spans="2:5" s="35" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B14" s="36"/>
-      <c r="C14" s="36"/>
+      <c r="C14" s="38"/>
       <c r="D14" s="36"/>
     </row>
     <row r="15" spans="2:5" s="35" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
IMPLEMENTACION DE METODOS Y SERVICIOS PARA CREAR CATEGORIA DE PRODUCTO || RETO 16 SERVICIOS VARIOS ||funciona ok
</commit_message>
<xml_diff>
--- a/Base de Datos/01DiseñoBDD.xlsx
+++ b/Base de Datos/01DiseñoBDD.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ESCUELAPROGRAMACIONKD\03MODULO\inventarios\Base de Datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DD4D54E-34B2-4398-9B15-B0675978E4C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEA9E54F-F99F-4A14-A89A-5D3A676BE47E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{E9E292EC-47DE-4FD1-BDC6-A5B6D9350F58}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="132">
   <si>
     <t>CATEGORIAS</t>
   </si>
@@ -418,6 +418,24 @@
   </si>
   <si>
     <t>actualiza o modifica un producto de acuerdo a la id</t>
+  </si>
+  <si>
+    <t>/categorias/crear</t>
+  </si>
+  <si>
+    <t>crea o inserta una nueva categoria en la tabla categoria</t>
+  </si>
+  <si>
+    <t>/categorias/actualizar</t>
+  </si>
+  <si>
+    <t>actualiza o modifica una categoria</t>
+  </si>
+  <si>
+    <t>/categorias/recuperar</t>
+  </si>
+  <si>
+    <t>recupera todas las categorias registradas en la tabla.</t>
   </si>
 </sst>
 </file>
@@ -1135,7 +1153,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6FBA827-0170-4345-A455-E7606A8500EF}">
   <dimension ref="B2:J75"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="A37" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="G61" sqref="G61"/>
     </sheetView>
   </sheetViews>
@@ -2081,12 +2099,12 @@
   <dimension ref="B2:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.42578125" customWidth="1"/>
+    <col min="1" max="1" width="4.28515625" customWidth="1"/>
     <col min="2" max="2" width="16.140625" style="33" customWidth="1"/>
     <col min="3" max="3" width="52.140625" style="33" customWidth="1"/>
     <col min="4" max="4" width="106.5703125" style="33" customWidth="1"/>
@@ -2210,19 +2228,37 @@
       </c>
     </row>
     <row r="13" spans="2:5" s="35" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B13" s="36"/>
-      <c r="C13" s="36"/>
-      <c r="D13" s="38"/>
+      <c r="B13" s="36" t="s">
+        <v>113</v>
+      </c>
+      <c r="C13" s="36" t="s">
+        <v>126</v>
+      </c>
+      <c r="D13" s="38" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="14" spans="2:5" s="35" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B14" s="36"/>
-      <c r="C14" s="38"/>
-      <c r="D14" s="36"/>
+      <c r="B14" s="36" t="s">
+        <v>117</v>
+      </c>
+      <c r="C14" s="36" t="s">
+        <v>128</v>
+      </c>
+      <c r="D14" s="36" t="s">
+        <v>129</v>
+      </c>
     </row>
     <row r="15" spans="2:5" s="35" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B15" s="36"/>
-      <c r="C15" s="36"/>
-      <c r="D15" s="36"/>
+      <c r="B15" s="36" t="s">
+        <v>102</v>
+      </c>
+      <c r="C15" s="36" t="s">
+        <v>130</v>
+      </c>
+      <c r="D15" s="36" t="s">
+        <v>131</v>
+      </c>
     </row>
     <row r="16" spans="2:5" s="35" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B16" s="36"/>

</xml_diff>

<commit_message>
IMPLEMENTACION DE METODOS Y SERVICIOS PARA RECUPERAR TODAS LAs CATEGORIA DE PRODUCTO || RETO 16 SERVICIOS VARIOS ||funciona ok
</commit_message>
<xml_diff>
--- a/Base de Datos/01DiseñoBDD.xlsx
+++ b/Base de Datos/01DiseñoBDD.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ESCUELAPROGRAMACIONKD\03MODULO\inventarios\Base de Datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEA9E54F-F99F-4A14-A89A-5D3A676BE47E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82CD2806-7FD2-49F4-AEB6-43A16E1F6204}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{E9E292EC-47DE-4FD1-BDC6-A5B6D9350F58}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="134">
   <si>
     <t>CATEGORIAS</t>
   </si>
@@ -436,6 +436,12 @@
   </si>
   <si>
     <t>recupera todas las categorias registradas en la tabla.</t>
+  </si>
+  <si>
+    <t>/pedidos/buscar/{identificadorProveedor]</t>
+  </si>
+  <si>
+    <t>Recupera los pedidos con sus respectivos detalles de un proveedor determinado. Recibe el identificador del proveedor.</t>
   </si>
 </sst>
 </file>
@@ -783,28 +789,28 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1170,11 +1176,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B2" s="39" t="s">
+      <c r="B2" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B3" s="8" t="s">
@@ -1265,15 +1271,15 @@
       </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C12" s="40" t="s">
+      <c r="C12" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="41"/>
+      <c r="D12" s="43"/>
       <c r="E12" s="42"/>
-      <c r="G12" s="39" t="s">
+      <c r="G12" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="H12" s="39"/>
+      <c r="H12" s="44"/>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C13" s="8" t="s">
@@ -1394,16 +1400,16 @@
       </c>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B23" s="45" t="s">
+      <c r="B23" s="39" t="s">
         <v>38</v>
       </c>
-      <c r="C23" s="46"/>
-      <c r="D23" s="46"/>
-      <c r="E23" s="46"/>
-      <c r="F23" s="46"/>
-      <c r="G23" s="46"/>
-      <c r="H23" s="46"/>
-      <c r="I23" s="46"/>
+      <c r="C23" s="40"/>
+      <c r="D23" s="40"/>
+      <c r="E23" s="40"/>
+      <c r="F23" s="40"/>
+      <c r="G23" s="40"/>
+      <c r="H23" s="40"/>
+      <c r="I23" s="40"/>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B24" s="8" t="s">
@@ -1536,10 +1542,10 @@
       </c>
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C31" s="39" t="s">
+      <c r="C31" s="44" t="s">
         <v>46</v>
       </c>
-      <c r="D31" s="39"/>
+      <c r="D31" s="44"/>
     </row>
     <row r="32" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C32" s="8" t="s">
@@ -1566,14 +1572,14 @@
       </c>
     </row>
     <row r="36" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B36" s="39" t="s">
+      <c r="B36" s="44" t="s">
         <v>50</v>
       </c>
-      <c r="C36" s="39"/>
-      <c r="D36" s="39"/>
-      <c r="E36" s="39"/>
-      <c r="F36" s="39"/>
-      <c r="G36" s="39"/>
+      <c r="C36" s="44"/>
+      <c r="D36" s="44"/>
+      <c r="E36" s="44"/>
+      <c r="F36" s="44"/>
+      <c r="G36" s="44"/>
     </row>
     <row r="37" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B37" s="8" t="s">
@@ -1636,13 +1642,13 @@
       </c>
     </row>
     <row r="42" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B42" s="43" t="s">
+      <c r="B42" s="45" t="s">
         <v>70</v>
       </c>
-      <c r="C42" s="44"/>
-      <c r="D42" s="44"/>
-      <c r="E42" s="44"/>
-      <c r="I42" s="40" t="s">
+      <c r="C42" s="46"/>
+      <c r="D42" s="46"/>
+      <c r="E42" s="46"/>
+      <c r="I42" s="41" t="s">
         <v>80</v>
       </c>
       <c r="J42" s="42"/>
@@ -1708,14 +1714,14 @@
       </c>
     </row>
     <row r="47" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B47" s="39" t="s">
+      <c r="B47" s="44" t="s">
         <v>71</v>
       </c>
-      <c r="C47" s="39"/>
-      <c r="D47" s="39"/>
-      <c r="E47" s="39"/>
-      <c r="F47" s="39"/>
-      <c r="G47" s="39"/>
+      <c r="C47" s="44"/>
+      <c r="D47" s="44"/>
+      <c r="E47" s="44"/>
+      <c r="F47" s="44"/>
+      <c r="G47" s="44"/>
     </row>
     <row r="48" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B48" s="8" t="s">
@@ -1806,12 +1812,12 @@
       <c r="G52" s="2"/>
     </row>
     <row r="54" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B54" s="40" t="s">
+      <c r="B54" s="41" t="s">
         <v>85</v>
       </c>
-      <c r="C54" s="41"/>
-      <c r="D54" s="41"/>
-      <c r="E54" s="41"/>
+      <c r="C54" s="43"/>
+      <c r="D54" s="43"/>
+      <c r="E54" s="43"/>
       <c r="F54" s="42"/>
     </row>
     <row r="55" spans="2:8" x14ac:dyDescent="0.25">
@@ -1926,12 +1932,12 @@
       </c>
     </row>
     <row r="64" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B64" s="40" t="s">
+      <c r="B64" s="41" t="s">
         <v>90</v>
       </c>
-      <c r="C64" s="41"/>
-      <c r="D64" s="41"/>
-      <c r="E64" s="41"/>
+      <c r="C64" s="43"/>
+      <c r="D64" s="43"/>
+      <c r="E64" s="43"/>
       <c r="F64" s="42"/>
     </row>
     <row r="65" spans="2:9" x14ac:dyDescent="0.25">
@@ -1969,15 +1975,15 @@
       </c>
     </row>
     <row r="69" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B69" s="45" t="s">
+      <c r="B69" s="39" t="s">
         <v>94</v>
       </c>
-      <c r="C69" s="46"/>
-      <c r="D69" s="46"/>
-      <c r="E69" s="46"/>
-      <c r="F69" s="46"/>
-      <c r="G69" s="46"/>
-      <c r="H69" s="46"/>
+      <c r="C69" s="40"/>
+      <c r="D69" s="40"/>
+      <c r="E69" s="40"/>
+      <c r="F69" s="40"/>
+      <c r="G69" s="40"/>
+      <c r="H69" s="40"/>
     </row>
     <row r="70" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B70" s="8" t="s">
@@ -2071,6 +2077,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="C12:E12"/>
+    <mergeCell ref="B47:G47"/>
+    <mergeCell ref="B42:E42"/>
     <mergeCell ref="B69:H69"/>
     <mergeCell ref="I42:J42"/>
     <mergeCell ref="B23:I23"/>
@@ -2078,11 +2089,6 @@
     <mergeCell ref="B64:F64"/>
     <mergeCell ref="C31:D31"/>
     <mergeCell ref="B36:G36"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="C12:E12"/>
-    <mergeCell ref="B47:G47"/>
-    <mergeCell ref="B42:E42"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
@@ -2099,7 +2105,7 @@
   <dimension ref="B2:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2107,7 +2113,7 @@
     <col min="1" max="1" width="4.28515625" customWidth="1"/>
     <col min="2" max="2" width="16.140625" style="33" customWidth="1"/>
     <col min="3" max="3" width="52.140625" style="33" customWidth="1"/>
-    <col min="4" max="4" width="106.5703125" style="33" customWidth="1"/>
+    <col min="4" max="4" width="138.85546875" style="33" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:5" s="35" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
@@ -2261,9 +2267,15 @@
       </c>
     </row>
     <row r="16" spans="2:5" s="35" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B16" s="36"/>
-      <c r="C16" s="36"/>
-      <c r="D16" s="36"/>
+      <c r="B16" s="36" t="s">
+        <v>102</v>
+      </c>
+      <c r="C16" s="36" t="s">
+        <v>132</v>
+      </c>
+      <c r="D16" s="36" t="s">
+        <v>133</v>
+      </c>
       <c r="E16" s="37"/>
     </row>
     <row r="17" spans="2:4" s="35" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">

</xml_diff>